<commit_message>
Updated sceneration output to simulation input method
Signed-off-by: Aytug Yavuzer <aytug.yavuzer@rwth-aachen.de>
</commit_message>
<xml_diff>
--- a/tutorials/simulations/sceneration/statistical_output.xlsx
+++ b/tutorials/simulations/sceneration/statistical_output.xlsx
@@ -40,31 +40,31 @@
     <t>MaxFastChargingPower</t>
   </si>
   <si>
+    <t>kia niro ev</t>
+  </si>
+  <si>
+    <t>audi e-tron gt rs</t>
+  </si>
+  <si>
+    <t>tesla y long range</t>
+  </si>
+  <si>
+    <t>renault megane e-tech ev60 220hp</t>
+  </si>
+  <si>
+    <t>kia ev6 gt</t>
+  </si>
+  <si>
     <t>bmw i4 edrive40</t>
   </si>
   <si>
-    <t>tesla y long range</t>
-  </si>
-  <si>
     <t>mercedes eqs 580 4matic</t>
   </si>
   <si>
     <t>mercedes eqe 350+</t>
   </si>
   <si>
-    <t>tesla s long range</t>
-  </si>
-  <si>
-    <t>bmw ix xdrive40</t>
-  </si>
-  <si>
-    <t>mercedes eqs 450+</t>
-  </si>
-  <si>
-    <t>renault megane e-tech ev60 220hp</t>
-  </si>
-  <si>
-    <t>tesla 3 long range</t>
+    <t>bmw i4 m50</t>
   </si>
 </sst>
 </file>
@@ -463,28 +463,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>44348.34375</v>
+        <v>44348.41666666666</v>
       </c>
       <c r="C2" s="2">
-        <v>44348.70833333334</v>
+        <v>44349.46875</v>
       </c>
       <c r="D2">
-        <v>0.648</v>
+        <v>0.44</v>
       </c>
       <c r="E2">
-        <v>0.773</v>
+        <v>0.861</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
       </c>
       <c r="G2">
-        <v>80.7</v>
+        <v>64.8</v>
       </c>
       <c r="H2">
         <v>11</v>
       </c>
       <c r="I2">
-        <v>200</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -492,28 +492,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>44348.46875</v>
+        <v>44348.41666666666</v>
       </c>
       <c r="C3" s="2">
-        <v>44348.72916666666</v>
+        <v>44348.69791666666</v>
       </c>
       <c r="D3">
-        <v>0.603</v>
+        <v>0.425</v>
       </c>
       <c r="E3">
-        <v>0.6950000000000001</v>
+        <v>0.658</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3">
-        <v>75</v>
+        <v>64.8</v>
       </c>
       <c r="H3">
         <v>11</v>
       </c>
       <c r="I3">
-        <v>250</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -521,28 +521,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>44348.34375</v>
+        <v>44348.35416666666</v>
       </c>
       <c r="C4" s="2">
-        <v>44348.77083333334</v>
+        <v>44349.6875</v>
       </c>
       <c r="D4">
-        <v>0.5</v>
+        <v>0.401</v>
       </c>
       <c r="E4">
-        <v>0.8280000000000001</v>
+        <v>0.802</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4">
-        <v>107.8</v>
+        <v>85</v>
       </c>
       <c r="H4">
         <v>11</v>
       </c>
       <c r="I4">
-        <v>207</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -550,28 +550,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>44348.32291666666</v>
+        <v>44348.4375</v>
       </c>
       <c r="C5" s="2">
-        <v>44348.71875</v>
+        <v>44349.71875</v>
       </c>
       <c r="D5">
-        <v>0.424</v>
+        <v>0.495</v>
       </c>
       <c r="E5">
-        <v>0.858</v>
+        <v>0.8470000000000001</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
       </c>
       <c r="G5">
-        <v>107.8</v>
+        <v>75</v>
       </c>
       <c r="H5">
         <v>11</v>
       </c>
       <c r="I5">
-        <v>207</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -579,28 +579,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>44348.30208333334</v>
+        <v>44348.58333333334</v>
       </c>
       <c r="C6" s="2">
-        <v>44349.48958333334</v>
+        <v>44349.76041666666</v>
       </c>
       <c r="D6">
-        <v>0.544</v>
+        <v>0.377</v>
       </c>
       <c r="E6">
-        <v>0.756</v>
+        <v>0.672</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
       </c>
       <c r="G6">
-        <v>90.59999999999999</v>
+        <v>60</v>
       </c>
       <c r="H6">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="I6">
-        <v>170</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -608,28 +608,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>44349.32291666666</v>
+        <v>44349.48958333334</v>
       </c>
       <c r="C7" s="2">
         <v>44350</v>
       </c>
       <c r="D7">
-        <v>0.623</v>
+        <v>0.421</v>
       </c>
       <c r="E7">
-        <v>0.8340000000000001</v>
+        <v>0.628</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
       </c>
       <c r="G7">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="H7">
-        <v>16.5</v>
+        <v>11</v>
       </c>
       <c r="I7">
-        <v>250</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -637,28 +637,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>44349.60416666666</v>
+        <v>44349.34375</v>
       </c>
       <c r="C8" s="2">
-        <v>44349.65625</v>
+        <v>44349.77083333334</v>
       </c>
       <c r="D8">
-        <v>0.387</v>
+        <v>0.5940000000000001</v>
       </c>
       <c r="E8">
-        <v>0.8330000000000001</v>
+        <v>0.8390000000000001</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
       </c>
       <c r="G8">
-        <v>71</v>
+        <v>80.7</v>
       </c>
       <c r="H8">
         <v>11</v>
       </c>
       <c r="I8">
-        <v>149</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -666,16 +666,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>44349.25</v>
+        <v>44349.35416666666</v>
       </c>
       <c r="C9" s="2">
-        <v>44350</v>
+        <v>44349.86458333334</v>
       </c>
       <c r="D9">
-        <v>0.417</v>
+        <v>0.36</v>
       </c>
       <c r="E9">
-        <v>0.8120000000000001</v>
+        <v>0.8070000000000001</v>
       </c>
       <c r="F9" t="s">
         <v>14</v>
@@ -695,28 +695,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>44349.29166666666</v>
+        <v>44349.36458333334</v>
       </c>
       <c r="C10" s="2">
-        <v>44349.71875</v>
+        <v>44350</v>
       </c>
       <c r="D10">
-        <v>0.429</v>
+        <v>0.492</v>
       </c>
       <c r="E10">
-        <v>0.736</v>
+        <v>0.8320000000000001</v>
       </c>
       <c r="F10" t="s">
         <v>15</v>
       </c>
       <c r="G10">
-        <v>60</v>
+        <v>90.59999999999999</v>
       </c>
       <c r="H10">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="I10">
-        <v>130</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -724,28 +724,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>44349.32291666666</v>
+        <v>44349.03125</v>
       </c>
       <c r="C11" s="2">
         <v>44350</v>
       </c>
       <c r="D11">
-        <v>0.392</v>
+        <v>0.438</v>
       </c>
       <c r="E11">
-        <v>0.773</v>
+        <v>0.5860000000000001</v>
       </c>
       <c r="F11" t="s">
         <v>16</v>
       </c>
       <c r="G11">
-        <v>75</v>
+        <v>80.7</v>
       </c>
       <c r="H11">
         <v>11</v>
       </c>
       <c r="I11">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>